<commit_message>
Dodanie pliku excel nwm w sumie po co xd
</commit_message>
<xml_diff>
--- a/Dzienniczek.xlsx
+++ b/Dzienniczek.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2398" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2406" uniqueCount="131">
   <si>
     <t>Lp</t>
   </si>
@@ -423,6 +423,24 @@
   <si>
     <t>24.2.2023</t>
   </si>
+  <si>
+    <t>GDFFGD</t>
+  </si>
+  <si>
+    <t>5.3.2023</t>
+  </si>
+  <si>
+    <t>dsaa</t>
+  </si>
+  <si>
+    <t>bvhbvjhvb</t>
+  </si>
+  <si>
+    <t>jh</t>
+  </si>
+  <si>
+    <t>9.3.2023</t>
+  </si>
 </sst>
 </file>
 
@@ -770,7 +788,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1027,6 +1045,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyAlignment="true" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -11268,8 +11298,8 @@
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A1" s="19"/>
-      <c r="B1" s="103" t="s">
-        <v>121</v>
+      <c r="B1" s="105" t="s">
+        <v>123</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -13615,7 +13645,9 @@
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A1" s="19"/>
-      <c r="B1" s="3"/>
+      <c r="B1" s="107" t="s">
+        <v>127</v>
+      </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="15" t="s">

</xml_diff>